<commit_message>
Clear code for compilation
</commit_message>
<xml_diff>
--- a/results/result.xlsx
+++ b/results/result.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
Correct routes for containers
</commit_message>
<xml_diff>
--- a/results/result.xlsx
+++ b/results/result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -562,7 +562,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">П-834 / Нижний Новгород г., 1-й Кемеровский пер.2; П-13 / Нижний Новгород г., 2-й Осташковский пер.1; П-325 / Нижний Новгород г., 30 лет Октября ул.2; П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2; П-326 / Нижний Новгород г., 40 лет Октября ул.15к1; П-331 / Нижний Новгород г., 40 лет Октября ул.26/1; П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б; П-696 / Нижний Новгород г., 40 лет Победы ул.1; </t>
+          <t xml:space="preserve">П-834 / Нижний Новгород г., 1-й Кемеровский пер.2; П-13 / Нижний Новгород г., 2-й Осташковский пер.1; П-325 / Нижний Новгород г., 30 лет Октября ул.2; П-331 / Нижний Новгород г., 40 лет Октября ул.26/1; П-696 / Нижний Новгород г., 40 лет Победы ул.1; </t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -577,22 +577,22 @@
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I2" t="n">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="J2" t="n">
-        <v>3682.8</v>
+        <v>2250.6</v>
       </c>
       <c r="K2" t="n">
-        <v>39.6</v>
+        <v>24.2</v>
       </c>
       <c r="L2" t="n">
         <v>32.90739535665041</v>
       </c>
       <c r="M2" t="n">
-        <v>22.63091772669362</v>
+        <v>19.40176032355866</v>
       </c>
       <c r="N2" t="n">
         <v>33.13107679041349</v>
@@ -604,25 +604,25 @@
         <v>26</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.6</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="R2" t="n">
         <v>0.4333333333333333</v>
       </c>
       <c r="S2" t="n">
-        <v>2.45231532927596</v>
+        <v>2.290857459119211</v>
       </c>
       <c r="T2" t="n">
-        <v>3.485648662609293</v>
+        <v>3.090857459119212</v>
       </c>
       <c r="U2" t="n">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="V2" t="n">
-        <v>88.66938987375752</v>
+        <v>85.44023247062256</v>
       </c>
       <c r="W2" t="n">
-        <v>209.1389197565576</v>
+        <v>185.4514475471527</v>
       </c>
     </row>
     <row r="3">
@@ -712,68 +712,293 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">П-834 / Нижний Новгород г., 1-й Кемеровский пер.2; П-13 / Нижний Новгород г., 2-й Осташковский пер.1; П-325 / Нижний Новгород г., 30 лет Октября ул.2; П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2; П-328 / Нижний Новгород г., 40 лет Октября ул.1А; П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б; П-696 / Нижний Новгород г., 40 лет Победы ул.1; </t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>КГМ</t>
-        </is>
+          <t>П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>8</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>КАМАЗ 43255-6010-69 (самосвал)</t>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>51.04008224844402</v>
+        <v>744</v>
       </c>
       <c r="K4" t="n">
-        <v>0.5488180886929465</v>
+        <v>8</v>
       </c>
       <c r="L4" t="n">
-        <v>32.90739535665041</v>
+        <v>34.38357677950807</v>
       </c>
       <c r="M4" t="n">
-        <v>22.33091772669363</v>
+        <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>33.13107679041349</v>
+        <v>34.38357677950807</v>
       </c>
       <c r="O4" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="P4" t="n">
         <v>15</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.35</v>
+        <v>0.25</v>
       </c>
       <c r="R4" t="n">
         <v>0.25</v>
       </c>
       <c r="S4" t="n">
+        <v>1.146119225983603</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1.646119225983603</v>
+      </c>
+      <c r="U4" t="n">
+        <v>30</v>
+      </c>
+      <c r="V4" t="n">
+        <v>68.76715355901614</v>
+      </c>
+      <c r="W4" t="n">
+        <v>98.76715355901615</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>П-326 / Нижний Новгород г., 40 лет Октября ул.15к1</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>8</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>744</v>
+      </c>
+      <c r="K5" t="n">
+        <v>8</v>
+      </c>
+      <c r="L5" t="n">
+        <v>34.38357677950807</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>34.38357677950807</v>
+      </c>
+      <c r="O5" t="n">
+        <v>40</v>
+      </c>
+      <c r="P5" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1.146119225983603</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1.646119225983603</v>
+      </c>
+      <c r="U5" t="n">
+        <v>30</v>
+      </c>
+      <c r="V5" t="n">
+        <v>68.76715355901614</v>
+      </c>
+      <c r="W5" t="n">
+        <v>98.76715355901615</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>8</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" t="n">
+        <v>744</v>
+      </c>
+      <c r="K6" t="n">
+        <v>8</v>
+      </c>
+      <c r="L6" t="n">
+        <v>34.38357677950807</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>34.38357677950807</v>
+      </c>
+      <c r="O6" t="n">
+        <v>40</v>
+      </c>
+      <c r="P6" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S6" t="n">
+        <v>1.146119225983603</v>
+      </c>
+      <c r="T6" t="n">
+        <v>1.646119225983603</v>
+      </c>
+      <c r="U6" t="n">
+        <v>30</v>
+      </c>
+      <c r="V6" t="n">
+        <v>68.76715355901614</v>
+      </c>
+      <c r="W6" t="n">
+        <v>98.76715355901615</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">П-834 / Нижний Новгород г., 1-й Кемеровский пер.2; П-13 / Нижний Новгород г., 2-й Осташковский пер.1; П-325 / Нижний Новгород г., 30 лет Октября ул.2; П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2; П-328 / Нижний Новгород г., 40 лет Октября ул.1А; П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б; П-696 / Нижний Новгород г., 40 лет Победы ул.1; </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>КГМ</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-6010-69 (самосвал)</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>5</v>
+      </c>
+      <c r="H7" t="n">
+        <v>7</v>
+      </c>
+      <c r="I7" t="n">
+        <v>7</v>
+      </c>
+      <c r="J7" t="n">
+        <v>51.04008224844402</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.5488180886929465</v>
+      </c>
+      <c r="L7" t="n">
+        <v>32.90739535665041</v>
+      </c>
+      <c r="M7" t="n">
+        <v>22.33091772669363</v>
+      </c>
+      <c r="N7" t="n">
+        <v>33.13107679041349</v>
+      </c>
+      <c r="O7" t="n">
+        <v>35</v>
+      </c>
+      <c r="P7" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S7" t="n">
         <v>2.43731532927596</v>
       </c>
-      <c r="T4" t="n">
+      <c r="T7" t="n">
         <v>3.03731532927596</v>
       </c>
-      <c r="U4" t="n">
+      <c r="U7" t="n">
         <v>36</v>
       </c>
-      <c r="V4" t="n">
+      <c r="V7" t="n">
         <v>88.36938987375753</v>
       </c>
-      <c r="W4" t="n">
+      <c r="W7" t="n">
         <v>182.2389197565576</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start to make optimized routes
</commit_message>
<xml_diff>
--- a/results/result.xlsx
+++ b/results/result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,13 +589,13 @@
         <v>24.2</v>
       </c>
       <c r="L2" t="n">
-        <v>32.90739535665041</v>
+        <v>24</v>
       </c>
       <c r="M2" t="n">
-        <v>19.40176032355866</v>
+        <v>26.55214770594985</v>
       </c>
       <c r="N2" t="n">
-        <v>33.13107679041349</v>
+        <v>24</v>
       </c>
       <c r="O2" t="n">
         <v>35</v>
@@ -610,19 +610,19 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="S2" t="n">
-        <v>2.290857459119211</v>
+        <v>2.287607385297493</v>
       </c>
       <c r="T2" t="n">
-        <v>3.090857459119212</v>
+        <v>3.087607385297493</v>
       </c>
       <c r="U2" t="n">
         <v>48</v>
       </c>
       <c r="V2" t="n">
-        <v>85.44023247062256</v>
+        <v>74.55214770594985</v>
       </c>
       <c r="W2" t="n">
-        <v>185.4514475471527</v>
+        <v>185.2564431178496</v>
       </c>
     </row>
     <row r="3">
@@ -664,13 +664,13 @@
         <v>1.5</v>
       </c>
       <c r="L3" t="n">
-        <v>34.52582305671596</v>
+        <v>24</v>
       </c>
       <c r="M3" t="n">
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>34.52582305671596</v>
+        <v>24</v>
       </c>
       <c r="O3" t="n">
         <v>35</v>
@@ -685,19 +685,19 @@
         <v>0.4333333333333333</v>
       </c>
       <c r="S3" t="n">
-        <v>1.381032922268639</v>
+        <v>0.9599999999999999</v>
       </c>
       <c r="T3" t="n">
-        <v>1.847699588935305</v>
+        <v>1.426666666666667</v>
       </c>
       <c r="U3" t="n">
         <v>28</v>
       </c>
       <c r="V3" t="n">
-        <v>69.05164611343193</v>
+        <v>48</v>
       </c>
       <c r="W3" t="n">
-        <v>110.8619753361183</v>
+        <v>85.59999999999999</v>
       </c>
     </row>
     <row r="4">
@@ -739,13 +739,13 @@
         <v>8</v>
       </c>
       <c r="L4" t="n">
-        <v>34.38357677950807</v>
+        <v>24</v>
       </c>
       <c r="M4" t="n">
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>34.38357677950807</v>
+        <v>24</v>
       </c>
       <c r="O4" t="n">
         <v>40</v>
@@ -760,19 +760,19 @@
         <v>0.25</v>
       </c>
       <c r="S4" t="n">
-        <v>1.146119225983603</v>
+        <v>0.8</v>
       </c>
       <c r="T4" t="n">
-        <v>1.646119225983603</v>
+        <v>1.3</v>
       </c>
       <c r="U4" t="n">
         <v>30</v>
       </c>
       <c r="V4" t="n">
-        <v>68.76715355901614</v>
+        <v>48</v>
       </c>
       <c r="W4" t="n">
-        <v>98.76715355901615</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5">
@@ -787,7 +787,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>П-326 / Нижний Новгород г., 40 лет Октября ул.15к1</t>
+          <t>П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2</t>
         </is>
       </c>
       <c r="E5" t="n">
@@ -814,13 +814,13 @@
         <v>8</v>
       </c>
       <c r="L5" t="n">
-        <v>34.38357677950807</v>
+        <v>24</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>34.38357677950807</v>
+        <v>24</v>
       </c>
       <c r="O5" t="n">
         <v>40</v>
@@ -835,19 +835,19 @@
         <v>0.25</v>
       </c>
       <c r="S5" t="n">
-        <v>1.146119225983603</v>
+        <v>0.8</v>
       </c>
       <c r="T5" t="n">
-        <v>1.646119225983603</v>
+        <v>1.3</v>
       </c>
       <c r="U5" t="n">
         <v>30</v>
       </c>
       <c r="V5" t="n">
-        <v>68.76715355901614</v>
+        <v>48</v>
       </c>
       <c r="W5" t="n">
-        <v>98.76715355901615</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6">
@@ -862,7 +862,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б</t>
+          <t>П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2</t>
         </is>
       </c>
       <c r="E6" t="n">
@@ -889,13 +889,13 @@
         <v>8</v>
       </c>
       <c r="L6" t="n">
-        <v>34.38357677950807</v>
+        <v>24</v>
       </c>
       <c r="M6" t="n">
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>34.38357677950807</v>
+        <v>24</v>
       </c>
       <c r="O6" t="n">
         <v>40</v>
@@ -910,19 +910,19 @@
         <v>0.25</v>
       </c>
       <c r="S6" t="n">
-        <v>1.146119225983603</v>
+        <v>0.8</v>
       </c>
       <c r="T6" t="n">
-        <v>1.646119225983603</v>
+        <v>1.3</v>
       </c>
       <c r="U6" t="n">
         <v>30</v>
       </c>
       <c r="V6" t="n">
-        <v>68.76715355901614</v>
+        <v>48</v>
       </c>
       <c r="W6" t="n">
-        <v>98.76715355901615</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
@@ -937,69 +937,894 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">П-834 / Нижний Новгород г., 1-й Кемеровский пер.2; П-13 / Нижний Новгород г., 2-й Осташковский пер.1; П-325 / Нижний Новгород г., 30 лет Октября ул.2; П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2; П-328 / Нижний Новгород г., 40 лет Октября ул.1А; П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б; П-696 / Нижний Новгород г., 40 лет Победы ул.1; </t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>КГМ</t>
-        </is>
+          <t>П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>КАМАЗ 43255-6010-69 (самосвал)</t>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H7" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
-        <v>51.04008224844402</v>
+        <v>744</v>
       </c>
       <c r="K7" t="n">
-        <v>0.5488180886929465</v>
+        <v>8</v>
       </c>
       <c r="L7" t="n">
-        <v>32.90739535665041</v>
+        <v>24</v>
       </c>
       <c r="M7" t="n">
-        <v>22.33091772669363</v>
+        <v>0</v>
       </c>
       <c r="N7" t="n">
-        <v>33.13107679041349</v>
+        <v>24</v>
       </c>
       <c r="O7" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="P7" t="n">
         <v>15</v>
       </c>
       <c r="Q7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T7" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U7" t="n">
+        <v>30</v>
+      </c>
+      <c r="V7" t="n">
+        <v>48</v>
+      </c>
+      <c r="W7" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>8</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>3</v>
+      </c>
+      <c r="H8" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" t="n">
+        <v>744</v>
+      </c>
+      <c r="K8" t="n">
+        <v>8</v>
+      </c>
+      <c r="L8" t="n">
+        <v>24</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>24</v>
+      </c>
+      <c r="O8" t="n">
+        <v>40</v>
+      </c>
+      <c r="P8" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T8" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U8" t="n">
+        <v>30</v>
+      </c>
+      <c r="V8" t="n">
+        <v>48</v>
+      </c>
+      <c r="W8" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>3</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" t="n">
+        <v>744</v>
+      </c>
+      <c r="K9" t="n">
+        <v>8</v>
+      </c>
+      <c r="L9" t="n">
+        <v>24</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>24</v>
+      </c>
+      <c r="O9" t="n">
+        <v>40</v>
+      </c>
+      <c r="P9" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T9" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U9" t="n">
+        <v>30</v>
+      </c>
+      <c r="V9" t="n">
+        <v>48</v>
+      </c>
+      <c r="W9" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>П-326 / Нижний Новгород г., 40 лет Октября ул.15к1</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" t="n">
+        <v>744</v>
+      </c>
+      <c r="K10" t="n">
+        <v>8</v>
+      </c>
+      <c r="L10" t="n">
+        <v>24</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>24</v>
+      </c>
+      <c r="O10" t="n">
+        <v>40</v>
+      </c>
+      <c r="P10" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T10" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U10" t="n">
+        <v>30</v>
+      </c>
+      <c r="V10" t="n">
+        <v>48</v>
+      </c>
+      <c r="W10" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>П-326 / Нижний Новгород г., 40 лет Октября ул.15к1</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>8</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>3</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" t="n">
+        <v>744</v>
+      </c>
+      <c r="K11" t="n">
+        <v>8</v>
+      </c>
+      <c r="L11" t="n">
+        <v>24</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>24</v>
+      </c>
+      <c r="O11" t="n">
+        <v>40</v>
+      </c>
+      <c r="P11" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T11" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U11" t="n">
+        <v>30</v>
+      </c>
+      <c r="V11" t="n">
+        <v>48</v>
+      </c>
+      <c r="W11" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>П-326 / Нижний Новгород г., 40 лет Октября ул.15к1</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>8</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>3</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" t="n">
+        <v>744</v>
+      </c>
+      <c r="K12" t="n">
+        <v>8</v>
+      </c>
+      <c r="L12" t="n">
+        <v>24</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>24</v>
+      </c>
+      <c r="O12" t="n">
+        <v>40</v>
+      </c>
+      <c r="P12" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U12" t="n">
+        <v>30</v>
+      </c>
+      <c r="V12" t="n">
+        <v>48</v>
+      </c>
+      <c r="W12" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>8</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>3</v>
+      </c>
+      <c r="H13" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>744</v>
+      </c>
+      <c r="K13" t="n">
+        <v>8</v>
+      </c>
+      <c r="L13" t="n">
+        <v>24</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>24</v>
+      </c>
+      <c r="O13" t="n">
+        <v>40</v>
+      </c>
+      <c r="P13" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T13" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U13" t="n">
+        <v>30</v>
+      </c>
+      <c r="V13" t="n">
+        <v>48</v>
+      </c>
+      <c r="W13" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>8</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>3</v>
+      </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>744</v>
+      </c>
+      <c r="K14" t="n">
+        <v>8</v>
+      </c>
+      <c r="L14" t="n">
+        <v>24</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>24</v>
+      </c>
+      <c r="O14" t="n">
+        <v>40</v>
+      </c>
+      <c r="P14" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T14" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U14" t="n">
+        <v>30</v>
+      </c>
+      <c r="V14" t="n">
+        <v>48</v>
+      </c>
+      <c r="W14" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>8</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" t="n">
+        <v>744</v>
+      </c>
+      <c r="K15" t="n">
+        <v>8</v>
+      </c>
+      <c r="L15" t="n">
+        <v>24</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>24</v>
+      </c>
+      <c r="O15" t="n">
+        <v>40</v>
+      </c>
+      <c r="P15" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T15" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U15" t="n">
+        <v>30</v>
+      </c>
+      <c r="V15" t="n">
+        <v>48</v>
+      </c>
+      <c r="W15" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>8</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>744</v>
+      </c>
+      <c r="K16" t="n">
+        <v>8</v>
+      </c>
+      <c r="L16" t="n">
+        <v>24</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>24</v>
+      </c>
+      <c r="O16" t="n">
+        <v>40</v>
+      </c>
+      <c r="P16" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T16" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U16" t="n">
+        <v>30</v>
+      </c>
+      <c r="V16" t="n">
+        <v>48</v>
+      </c>
+      <c r="W16" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-3010-69, МК-4512-04</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>3</v>
+      </c>
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
+        <v>744</v>
+      </c>
+      <c r="K17" t="n">
+        <v>8</v>
+      </c>
+      <c r="L17" t="n">
+        <v>24</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>24</v>
+      </c>
+      <c r="O17" t="n">
+        <v>40</v>
+      </c>
+      <c r="P17" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="T17" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="U17" t="n">
+        <v>30</v>
+      </c>
+      <c r="V17" t="n">
+        <v>48</v>
+      </c>
+      <c r="W17" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>приокский район</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">П-834 / Нижний Новгород г., 1-й Кемеровский пер.2; П-13 / Нижний Новгород г., 2-й Осташковский пер.1; П-325 / Нижний Новгород г., 30 лет Октября ул.2; П-709 / Нижний Новгород г., 40 лет Октября ул.15 к2; П-328 / Нижний Новгород г., 40 лет Октября ул.1А; П-1260 / Нижний Новгород г., 40 лет Октября ул.7Б; П-696 / Нижний Новгород г., 40 лет Победы ул.1; </t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>КГМ</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>КАМАЗ 43255-6010-69 (самосвал)</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>5</v>
+      </c>
+      <c r="H18" t="n">
+        <v>7</v>
+      </c>
+      <c r="I18" t="n">
+        <v>7</v>
+      </c>
+      <c r="J18" t="n">
+        <v>51.04008224844402</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.5488180886929465</v>
+      </c>
+      <c r="L18" t="n">
+        <v>24</v>
+      </c>
+      <c r="M18" t="n">
+        <v>27.15214770594984</v>
+      </c>
+      <c r="N18" t="n">
+        <v>24</v>
+      </c>
+      <c r="O18" t="n">
+        <v>35</v>
+      </c>
+      <c r="P18" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q18" t="n">
         <v>0.35</v>
       </c>
-      <c r="R7" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="S7" t="n">
-        <v>2.43731532927596</v>
-      </c>
-      <c r="T7" t="n">
-        <v>3.03731532927596</v>
-      </c>
-      <c r="U7" t="n">
+      <c r="R18" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="S18" t="n">
+        <v>2.317607385297493</v>
+      </c>
+      <c r="T18" t="n">
+        <v>2.917607385297493</v>
+      </c>
+      <c r="U18" t="n">
         <v>36</v>
       </c>
-      <c r="V7" t="n">
-        <v>88.36938987375753</v>
-      </c>
-      <c r="W7" t="n">
-        <v>182.2389197565576</v>
+      <c r="V18" t="n">
+        <v>75.15214770594984</v>
+      </c>
+      <c r="W18" t="n">
+        <v>175.0564431178496</v>
       </c>
     </row>
   </sheetData>

</xml_diff>